<commit_message>
fix typo in requirements document
</commit_message>
<xml_diff>
--- a/deliverables/deliverables-sprint2/cs4320-terrapins-requirements.xlsx
+++ b/deliverables/deliverables-sprint2/cs4320-terrapins-requirements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/zhoue_umsystem_edu/Documents/SP2022/CS4320/Final Project/Sprint 1/Deliverables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/zhoue_umsystem_edu/Documents/SP2022/CS4320/CS4320 Final Project/Sprint 2/Deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{EC2A865C-B1C9-FE4C-AADD-85B4018B2360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D12F881-9691-46FF-9F7B-CBA418EFCEF9}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="8_{EC2A865C-B1C9-FE4C-AADD-85B4018B2360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C73E6D3-BC55-4BDA-A693-111082080EF9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E56C6C9A-C3BB-8C46-86E5-B995A5932795}"/>
   </bookViews>
@@ -62,9 +62,6 @@
     <t>API server endpoint should work with reasonable reliability</t>
   </si>
   <si>
-    <t>Graph Initalization</t>
-  </si>
-  <si>
     <t>Data drawn out of API endpoint will be visualized in graph form that can be fed into graphic software.</t>
   </si>
   <si>
@@ -228,6 +225,9 @@
   </si>
   <si>
     <t>Logged in user can specify shipping address for each item</t>
+  </si>
+  <si>
+    <t>Graph Initialization</t>
   </si>
 </sst>
 </file>
@@ -612,19 +612,19 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="20" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="53.5546875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.77734375" style="2"/>
+    <col min="3" max="3" width="33.36328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="53.54296875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.15" customHeight="1">
+    <row r="1" spans="1:4" ht="22.2" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -638,7 +638,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -652,7 +652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="36">
+    <row r="3" spans="1:4" ht="30">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -660,66 +660,66 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="30">
+      <c r="A4" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="36">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="36">
+    </row>
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="30">
+      <c r="A6" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="36">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17.25">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -735,12 +735,12 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="2"/>
+    <col min="2" max="2" width="10.81640625" style="2"/>
     <col min="3" max="3" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.81640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.6">
@@ -748,7 +748,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -759,268 +759,268 @@
     </row>
     <row r="2" spans="1:4" ht="45">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="105">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="60">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="60">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="75">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="60">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="60">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="60">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1">
         <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="75">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1">
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="1">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="1">
         <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>